<commit_message>
evaluation excluding exact matches
</commit_message>
<xml_diff>
--- a/evaluate_macthing.xlsx
+++ b/evaluate_macthing.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Projects/KGEntityMatching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04172E8-AF63-8B49-90DB-89120DD9ACEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6247BABC-E4AA-3643-8A54-65C9103141CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{621E5187-92B8-5C43-8683-AF9FDC089AB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>big-small comm-comm</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Gold pairs in matched top 10</t>
+  </si>
+  <si>
+    <t>Gold pairs (-exact) in matched top 1</t>
+  </si>
+  <si>
+    <t>Gold pairs (-exact) in matched top 5</t>
+  </si>
+  <si>
+    <t>Gold pairs (-exact) in matched top 10</t>
   </si>
 </sst>
 </file>
@@ -64,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,6 +84,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,13 +437,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C626804-5724-3A4A-B1FB-2F083E4C0C8F}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="2" max="3" width="20.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -498,4 +515,88 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991ADE54-B857-034A-9F0C-F258E5C00738}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.18243243243243201</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.18918918918918901</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.195945945945945</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.18918918918918901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.22972972972972899</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.23648648648648599</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.37837837837837801</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.35135135135135098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.27702702702702697</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.28378378378378299</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.46621621621621601</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.445945945945946</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated some code for overlapping communities
</commit_message>
<xml_diff>
--- a/evaluate_macthing.xlsx
+++ b/evaluate_macthing.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Projects/KGEntityMatching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6247BABC-E4AA-3643-8A54-65C9103141CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0333C2C-A454-0A48-9F2F-7BF1BE08B03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{621E5187-92B8-5C43-8683-AF9FDC089AB2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" activeTab="3" xr2:uid="{621E5187-92B8-5C43-8683-AF9FDC089AB2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="leiden_f gold" sheetId="1" r:id="rId1"/>
+    <sheet name="leiden_f_goldnotexact" sheetId="2" r:id="rId2"/>
+    <sheet name="leiden_0_gold" sheetId="4" r:id="rId3"/>
+    <sheet name="leiden_0_goldnotexact" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>big-small comm-comm</t>
   </si>
@@ -437,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C626804-5724-3A4A-B1FB-2F083E4C0C8F}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -521,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991ADE54-B857-034A-9F0C-F258E5C00738}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -599,4 +601,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73EFC40-7E74-844E-A030-A7C8DA676E35}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEC326B-DD7A-E24E-B1EA-158A60D2FF5A}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3">
+        <v>0.31756756756756699</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.43243243243243201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.91216216216216195</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>